<commit_message>
move calculation train cycle to the class TimetableLine
</commit_message>
<xml_diff>
--- a/example_data/import/subproject_bvwp.xlsx
+++ b/example_data/import/subproject_bvwp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/PycharmProjects/pros/example_data/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86930AB-FE06-8540-987B-DF799FC1DADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FECAAF-B0E2-094F-9654-7E4DEF977C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="11760" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deutschlandtakt" sheetId="4" r:id="rId1"/>
@@ -20,8 +20,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Noch nicht in qgis" guid="{88289622-D034-4E38-A0C0-61CEB0F9C67E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="NKV &lt; 1,5" guid="{23E76F66-981C-4206-9E06-CBB72D7DAC5B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Noch nicht in qgis" guid="{88289622-D034-4E38-A0C0-61CEB0F9C67E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="297">
   <si>
     <t>nbs</t>
   </si>
@@ -700,6 +700,237 @@
   </si>
   <si>
     <t>Kreuzungsgleise in Raddusch und Kunersdorf</t>
+  </si>
+  <si>
+    <t>2-030-V01 TM1</t>
+  </si>
+  <si>
+    <t>Elektrifizierung Gotha – Leinefelde und Geschwindigkeitserhöhung, Streckenklasse D4</t>
+  </si>
+  <si>
+    <t>2-030-V01 TM2</t>
+  </si>
+  <si>
+    <t>Verbindungskurve Gotha, vmax 70 km/h</t>
+  </si>
+  <si>
+    <t>2-030-V01 TM3</t>
+  </si>
+  <si>
+    <t>Kreuzungsbahnhöfe in Ballstädt, Mühlhausen und Silberhausen</t>
+  </si>
+  <si>
+    <t>2-007-V01 TM1</t>
+  </si>
+  <si>
+    <t>ABS/NBS Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach Teilmaßnahme Hanau – Gelnhausen</t>
+  </si>
+  <si>
+    <t>ABS Gotha - Leinefelde Teilmaßnahmen Elektrifizierung und Geschwindigkeitserhöhung</t>
+  </si>
+  <si>
+    <t>ABS Gotha - Leinefelde Teilmaßnahmen Verbindungskurve Gotha</t>
+  </si>
+  <si>
+    <t>ABS Gotha - Leinefelde Teilmaßnahmen Kreuzungsbahnhöfe</t>
+  </si>
+  <si>
+    <t>Hanau – Gelnhausen 3. und 4. Gleis, vmax 200 km/h</t>
+  </si>
+  <si>
+    <t>2-007-V01 TM2</t>
+  </si>
+  <si>
+    <t>ABS/NBS Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach NBS Gelnhausen – Fulda</t>
+  </si>
+  <si>
+    <t>NBS Gelnhausen – Fulda mit Verbindungskurve zur 3600, höhenfreie Einbindung in SFS Fulda – Würzburg</t>
+  </si>
+  <si>
+    <t>2-007-V01 TM3</t>
+  </si>
+  <si>
+    <t>ABS/NBS Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach ABS/NBS Korridor Wildeck/Blankenheim – Bad Hersfeld – Kirchheim/Langenschwarz, 200 km/h</t>
+  </si>
+  <si>
+    <t>ABS/NBS Korridor Wildeck/Blankenheim – Bad Hersfeld – Kirchheim/Langenschwarz, vmax 200, höhenfreie Einbindung in die NBS Kassel – Fulda</t>
+  </si>
+  <si>
+    <t>ABS/NBS Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach Geschwindigkeitserhöhung Eisenach – Erfurt</t>
+  </si>
+  <si>
+    <t>2-007-V01 TM4</t>
+  </si>
+  <si>
+    <t>ABS/NBS Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach Blockverdichtung Aschaffenburg – Nantenbach</t>
+  </si>
+  <si>
+    <t>2-007-V01 TM5</t>
+  </si>
+  <si>
+    <t>vmax Eisenach – Erfurt 200 km/h</t>
+  </si>
+  <si>
+    <t>Blockverdichtung Aschaffenburg – Nantenbach</t>
+  </si>
+  <si>
+    <t>ABS Münster - Lünen Teilmaßnahme Geschwindigkeitserhöhung Werne – Münster</t>
+  </si>
+  <si>
+    <t>2-049-V02 TM1</t>
+  </si>
+  <si>
+    <t>Geschwindigkeitserhöhung Werne – Münster auf vmax 230</t>
+  </si>
+  <si>
+    <t>ABS Münster - Lünen Teilmaßnahme zweigleisiger Ausbau Capelle – Ascheberg</t>
+  </si>
+  <si>
+    <t>2-049-V02 TM2</t>
+  </si>
+  <si>
+    <t>zweigleisiger Ausbau Capelle – Ascheberg auf vmax 230</t>
+  </si>
+  <si>
+    <t>ABS Münster - Lünen Teilmaßnahme Kreuzungsbahnhof Münster-Amelsbüren und Davensberg</t>
+  </si>
+  <si>
+    <t>2-049-V02 TM3</t>
+  </si>
+  <si>
+    <t>Kreuzungsbahnhöfe Münster-Amelsbüren und Davensberg</t>
+  </si>
+  <si>
+    <t>ABS Grenze NL/D – Kaldenkirchen – Mönchengladbach – Rheydt-Odenkirchen Teilmaßnahme Kaldenkirchen – Dülken</t>
+  </si>
+  <si>
+    <t>2-025-V01 TM1</t>
+  </si>
+  <si>
+    <t>2. Gleis Kaldenkirchen – Dülken, vmax 120 km/h</t>
+  </si>
+  <si>
+    <t>ABS Grenze NL/D – Kaldenkirchen – Mönchengladbach – Rheydt-Odenkirchen Teilmaßnahme Rheydt – Rheydt-Odenkirchen</t>
+  </si>
+  <si>
+    <t>2-025-V01 TM2</t>
+  </si>
+  <si>
+    <t>zweites Gleis Rheydt – Rheydt-Odenkirchen</t>
+  </si>
+  <si>
+    <t>2-025-V01 TM3</t>
+  </si>
+  <si>
+    <t>Verbindungskurve Viersen, vmax = 60</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM1</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme NBS Zeppelinheim – Mannheim-Waldhof</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme Verbindungskurve Klein-Gerau/Weiterstadt/Griesheim</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM2</t>
+  </si>
+  <si>
+    <t>Verbindungskurve Klein-Gerau/Weiterstadt/Griesheim</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme zweites Gleis Mannheim Käfertal – Mannheim Rangierbahnhof</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM3</t>
+  </si>
+  <si>
+    <t>zweites Gleis Mannheim Käfertal – Mannheim</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme ABS/NBS Molzau – Graben-Neudorf – Karlsruhe</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM4</t>
+  </si>
+  <si>
+    <t>ABS/NBS Molzau – Graben-Neudorf – Karlsruhe</t>
+  </si>
+  <si>
+    <t>NBS Zeppelinheim – Mannheim-Waldhof, vmax 300 km/h, Verknüpfungen in Zeppelinheim, Mannheim-Waldhof, Weiterstadt/Griesheim, Darmstadt und Graben-Neudorf höhenfrei</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM5</t>
+  </si>
+  <si>
+    <t>eingleisige Verbindungskurve Wiesbadener und Frankfurter Ast der Schnellfahrstrecke Köln – Rhein/Main mit niveaugleicher Einfädelung in Frankfurter Ast (Wallauer Spange)</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme Wallauer Spange</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme drittes Gleis Karlsruhe – Durmersheim</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM6</t>
+  </si>
+  <si>
+    <t>drittes Gleis Karlsruhe – Durmersheim</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme drittes Gleis Groß Gerau-dornberg – Riedstadt-Goddelau</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM7</t>
+  </si>
+  <si>
+    <t>drittes Gleis Groß Gerau-Dornberg – Riedstadt-Goddelau</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM8</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme KV-Profil P/C 400 Hagen – Siegen Ost Gbf, Au – Siegen – Siegen Ost Gbf, Siegen – Siegen-Weidenau</t>
+  </si>
+  <si>
+    <t>KV-Profil P/C 400 Hagen – Siegen Ost Gbf, Au – Siegen – Siegen Ost Gbf, Siegen – Siegen-Weidenau</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme Blockverdichtung Krueztal – Siegen, Wetzlar – Gießen-Bergwald – Friedberg</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM9</t>
+  </si>
+  <si>
+    <t>Blockverdichtung Krueztal – Siegen, Wetzlar – Gießen-Bergwald – Friedberg</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme 10 zweites Gleis Blankenberg – Merten, Schladern – Rosbach</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM10</t>
+  </si>
+  <si>
+    <t>zweites Gleis Blankenberg – Merten, Schladern – Rosbach</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM11</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme 11 höhenfreie Verknüpfung Friedberg, Großkrotzenburg</t>
+  </si>
+  <si>
+    <t>höhenfreie Verknüpfung Friedberg, Großkrotzenburg</t>
+  </si>
+  <si>
+    <t>Korridor Mittelrhein: Zielnetz 1 Teilmaßnahme 12 viergleisiger Ausbau Frankfurt-Stadion – Zeppelinheim</t>
+  </si>
+  <si>
+    <t>2-004-V03 TM12</t>
+  </si>
+  <si>
+    <t>viergleisiger Ausbau Frankfurt-Stadion – Zeppelinheim inklusive Güterzuggleis Frankfurt Stadion</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1307,8 @@
   <dimension ref="A1:AX1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2398,7 +2629,7 @@
         <v>114</v>
       </c>
       <c r="E26" s="2" t="str">
-        <f t="shared" ref="E26:G34" si="1">RIGHT(C26,LEN(C26)-SEARCH(" ",C26,1))</f>
+        <f t="shared" ref="E26:G30" si="1">RIGHT(C26,LEN(C26)-SEARCH(" ",C26,1))</f>
         <v>Lübeck – Lüneburg Teilmaßnahme Elektrifizierung</v>
       </c>
       <c r="F26" s="2"/>
@@ -3029,7 +3260,7 @@
         <v>149</v>
       </c>
       <c r="E39" s="2" t="str">
-        <f t="shared" ref="E39:G62" si="2">RIGHT(C39,LEN(C39)-SEARCH(" ",C39,1))</f>
+        <f t="shared" ref="E39:G88" si="2">RIGHT(C39,LEN(C39)-SEARCH(" ",C39,1))</f>
         <v>Uelzen – Stendal - Magdeburg - Halle (Ostkorridor Nord) Teilmaßnahme Veerßen – Salzwedel</v>
       </c>
       <c r="F39" s="2"/>
@@ -4098,19 +4329,43 @@
       <c r="AW62" s="2"/>
       <c r="AX62" s="2"/>
     </row>
-    <row r="63" spans="1:50" ht="16">
+    <row r="63" spans="1:50" ht="68">
       <c r="A63" s="2"/>
       <c r="B63" s="3">
         <v>55</v>
       </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E63" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Gotha - Leinefelde Teilmaßnahmen Elektrifizierung und Geschwindigkeitserhöhung</v>
+      </c>
       <c r="F63" s="2"/>
-      <c r="G63" s="3"/>
+      <c r="G63" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="H63" s="3"/>
       <c r="I63" s="4"/>
       <c r="K63" s="1"/>
+      <c r="L63" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA63" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB63">
+        <v>160</v>
+      </c>
+      <c r="AK63" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL63" t="b">
+        <v>1</v>
+      </c>
       <c r="AO63" s="2"/>
       <c r="AP63" s="2"/>
       <c r="AQ63" s="4"/>
@@ -4122,16 +4377,42 @@
       <c r="AW63" s="2"/>
       <c r="AX63" s="2"/>
     </row>
-    <row r="64" spans="1:50" ht="16">
+    <row r="64" spans="1:50" ht="34">
       <c r="A64" s="2"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="B64" s="3">
+        <v>55</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E64" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Gotha - Leinefelde Teilmaßnahmen Verbindungskurve Gotha</v>
+      </c>
       <c r="F64" s="2"/>
-      <c r="G64" s="3"/>
+      <c r="G64" s="3" t="s">
+        <v>223</v>
+      </c>
       <c r="H64" s="3"/>
       <c r="I64" s="4"/>
+      <c r="L64" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA64" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB64">
+        <v>70</v>
+      </c>
+      <c r="AK64" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL64" t="b">
+        <v>1</v>
+      </c>
       <c r="AO64" s="2"/>
       <c r="AP64" s="2"/>
       <c r="AQ64" s="4"/>
@@ -4143,18 +4424,41 @@
       <c r="AW64" s="2"/>
       <c r="AX64" s="2"/>
     </row>
-    <row r="65" spans="1:50" ht="16">
+    <row r="65" spans="1:50" ht="34">
       <c r="A65" s="2"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="B65" s="3">
+        <v>55</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E65" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Gotha - Leinefelde Teilmaßnahmen Kreuzungsbahnhöfe</v>
+      </c>
       <c r="F65" s="2"/>
-      <c r="G65" s="3"/>
+      <c r="G65" s="3" t="s">
+        <v>225</v>
+      </c>
       <c r="H65" s="3"/>
       <c r="I65" s="4"/>
       <c r="R65" s="1"/>
+      <c r="S65" t="b">
+        <v>1</v>
+      </c>
+      <c r="T65">
+        <v>3</v>
+      </c>
       <c r="AF65" s="1"/>
+      <c r="AK65" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL65" t="b">
+        <v>1</v>
+      </c>
       <c r="AO65" s="2"/>
       <c r="AP65" s="2"/>
       <c r="AQ65" s="4"/>
@@ -4166,19 +4470,52 @@
       <c r="AW65" s="2"/>
       <c r="AX65" s="2"/>
     </row>
-    <row r="66" spans="1:50" ht="16">
+    <row r="66" spans="1:50" ht="34">
       <c r="A66" s="2"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="B66" s="3">
+        <v>56</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E66" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach Teilmaßnahme Hanau – Gelnhausen</v>
+      </c>
       <c r="F66" s="2"/>
-      <c r="G66" s="3"/>
+      <c r="G66" s="3" t="s">
+        <v>231</v>
+      </c>
       <c r="H66" s="3"/>
       <c r="I66" s="4"/>
       <c r="J66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
+      <c r="K66" t="b">
+        <v>1</v>
+      </c>
+      <c r="O66" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P66" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB66">
+        <v>200</v>
+      </c>
+      <c r="AJ66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL66" t="b">
+        <v>1</v>
+      </c>
       <c r="AO66" s="2"/>
       <c r="AP66" s="2"/>
       <c r="AQ66" s="4"/>
@@ -4190,18 +4527,47 @@
       <c r="AW66" s="2"/>
       <c r="AX66" s="2"/>
     </row>
-    <row r="67" spans="1:50" ht="16">
+    <row r="67" spans="1:50" ht="68">
       <c r="A67" s="2"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="B67" s="3">
+        <v>56</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E67" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach NBS Gelnhausen – Fulda</v>
+      </c>
       <c r="F67" s="2"/>
-      <c r="G67" s="3"/>
+      <c r="G67" s="3" t="s">
+        <v>234</v>
+      </c>
       <c r="H67" s="3"/>
       <c r="I67" s="4"/>
+      <c r="J67" t="b">
+        <v>1</v>
+      </c>
       <c r="K67" s="1"/>
       <c r="P67" s="1"/>
+      <c r="AA67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB67">
+        <v>200</v>
+      </c>
+      <c r="AJ67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL67" t="b">
+        <v>1</v>
+      </c>
       <c r="AO67" s="2"/>
       <c r="AP67" s="2"/>
       <c r="AQ67" s="4"/>
@@ -4213,17 +4579,49 @@
       <c r="AW67" s="2"/>
       <c r="AX67" s="2"/>
     </row>
-    <row r="68" spans="1:50" ht="16">
+    <row r="68" spans="1:50" ht="102">
       <c r="A68" s="2"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
+      <c r="B68" s="3">
+        <v>56</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E68" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach ABS/NBS Korridor Wildeck/Blankenheim – Bad Hersfeld – Kirchheim/Langenschwarz, 200 km/h</v>
+      </c>
       <c r="F68" s="2"/>
-      <c r="G68" s="3"/>
+      <c r="G68" s="3" t="s">
+        <v>237</v>
+      </c>
       <c r="H68" s="3"/>
       <c r="I68" s="4"/>
+      <c r="J68" t="b">
+        <v>1</v>
+      </c>
+      <c r="K68" t="b">
+        <v>1</v>
+      </c>
       <c r="R68" s="1"/>
+      <c r="AA68" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB68">
+        <v>200</v>
+      </c>
+      <c r="AJ68" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK68" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL68" t="b">
+        <v>1</v>
+      </c>
       <c r="AO68" s="2"/>
       <c r="AP68" s="2"/>
       <c r="AQ68" s="4"/>
@@ -4235,19 +4633,47 @@
       <c r="AW68" s="2"/>
       <c r="AX68" s="2"/>
     </row>
-    <row r="69" spans="1:50" ht="16">
+    <row r="69" spans="1:50" ht="17">
       <c r="A69" s="2"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
+      <c r="B69" s="3">
+        <v>56</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E69" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach Geschwindigkeitserhöhung Eisenach – Erfurt</v>
+      </c>
       <c r="F69" s="2"/>
-      <c r="G69" s="3"/>
+      <c r="G69" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="H69" s="3"/>
       <c r="I69" s="4"/>
-      <c r="K69" s="1"/>
+      <c r="K69" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="N69" s="1"/>
       <c r="S69" s="1"/>
+      <c r="AA69" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB69">
+        <v>200</v>
+      </c>
+      <c r="AJ69" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK69" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL69" t="b">
+        <v>1</v>
+      </c>
       <c r="AO69" s="2"/>
       <c r="AP69" s="2"/>
       <c r="AQ69" s="4"/>
@@ -4259,17 +4685,40 @@
       <c r="AW69" s="2"/>
       <c r="AX69" s="2"/>
     </row>
-    <row r="70" spans="1:50" ht="16">
+    <row r="70" spans="1:50" ht="34">
       <c r="A70" s="2"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
+      <c r="B70" s="3">
+        <v>56</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E70" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Hanau - Fulda - Erfurt / Aschaffenburg - Nantenbach Blockverdichtung Aschaffenburg – Nantenbach</v>
+      </c>
       <c r="F70" s="2"/>
-      <c r="G70" s="3"/>
+      <c r="G70" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="H70" s="3"/>
       <c r="I70" s="4"/>
+      <c r="X70" t="b">
+        <v>1</v>
+      </c>
       <c r="AF70" s="1"/>
+      <c r="AJ70" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK70" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL70" t="b">
+        <v>1</v>
+      </c>
       <c r="AO70" s="2"/>
       <c r="AP70" s="2"/>
       <c r="AQ70" s="5"/>
@@ -4281,17 +4730,46 @@
       <c r="AW70" s="2"/>
       <c r="AX70" s="2"/>
     </row>
-    <row r="71" spans="1:50" ht="16">
+    <row r="71" spans="1:50" ht="34">
       <c r="A71" s="2"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
+      <c r="B71" s="3">
+        <v>59</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E71" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Münster - Lünen Teilmaßnahme Geschwindigkeitserhöhung Werne – Münster</v>
+      </c>
       <c r="F71" s="2"/>
-      <c r="G71" s="3"/>
+      <c r="G71" s="3" t="s">
+        <v>246</v>
+      </c>
       <c r="H71" s="3"/>
       <c r="I71" s="4"/>
+      <c r="K71" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="Y71" s="1"/>
+      <c r="AA71" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB71">
+        <v>230</v>
+      </c>
+      <c r="AJ71" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK71" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL71" t="b">
+        <v>1</v>
+      </c>
       <c r="AO71" s="2"/>
       <c r="AP71" s="2"/>
       <c r="AQ71" s="5"/>
@@ -4303,19 +4781,50 @@
       <c r="AW71" s="2"/>
       <c r="AX71" s="2"/>
     </row>
-    <row r="72" spans="1:50" ht="16">
+    <row r="72" spans="1:50" ht="34">
       <c r="A72" s="2"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
+      <c r="B72" s="3">
+        <v>59</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E72" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Münster - Lünen Teilmaßnahme zweigleisiger Ausbau Capelle – Ascheberg</v>
+      </c>
       <c r="F72" s="2"/>
-      <c r="G72" s="3"/>
+      <c r="G72" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="H72" s="3"/>
       <c r="I72" s="4"/>
-      <c r="N72" s="1"/>
+      <c r="K72" t="b">
+        <v>1</v>
+      </c>
+      <c r="N72" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="P72" s="1"/>
       <c r="R72" s="1"/>
+      <c r="AA72" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB72">
+        <v>230</v>
+      </c>
+      <c r="AJ72" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK72" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL72" t="b">
+        <v>1</v>
+      </c>
       <c r="AO72" s="2"/>
       <c r="AP72" s="2"/>
       <c r="AQ72" s="5"/>
@@ -4327,18 +4836,44 @@
       <c r="AW72" s="2"/>
       <c r="AX72" s="2"/>
     </row>
-    <row r="73" spans="1:50" ht="16">
+    <row r="73" spans="1:50" ht="34">
       <c r="A73" s="2"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
+      <c r="B73" s="3">
+        <v>59</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E73" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Münster - Lünen Teilmaßnahme Kreuzungsbahnhof Münster-Amelsbüren und Davensberg</v>
+      </c>
       <c r="F73" s="2"/>
-      <c r="G73" s="3"/>
+      <c r="G73" s="3" t="s">
+        <v>252</v>
+      </c>
       <c r="H73" s="3"/>
       <c r="I73" s="4"/>
       <c r="N73" s="1"/>
+      <c r="S73" t="b">
+        <v>1</v>
+      </c>
+      <c r="T73">
+        <v>2</v>
+      </c>
       <c r="AF73" s="1"/>
+      <c r="AJ73" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK73" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL73" t="b">
+        <v>1</v>
+      </c>
       <c r="AO73" s="2"/>
       <c r="AP73" s="2"/>
       <c r="AQ73" s="4"/>
@@ -4350,17 +4885,43 @@
       <c r="AW73" s="2"/>
       <c r="AX73" s="2"/>
     </row>
-    <row r="74" spans="1:50" ht="16">
+    <row r="74" spans="1:50" ht="34">
       <c r="A74" s="2"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
+      <c r="B74" s="3">
+        <v>62</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E74" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Grenze NL/D – Kaldenkirchen – Mönchengladbach – Rheydt-Odenkirchen Teilmaßnahme Kaldenkirchen – Dülken</v>
+      </c>
       <c r="F74" s="2"/>
-      <c r="G74" s="3"/>
+      <c r="G74" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="H74" s="3"/>
       <c r="I74" s="4"/>
+      <c r="N74" t="b">
+        <v>1</v>
+      </c>
       <c r="S74" s="1"/>
+      <c r="AA74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB74">
+        <v>120</v>
+      </c>
+      <c r="AK74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL74" t="b">
+        <v>1</v>
+      </c>
       <c r="AO74" s="2"/>
       <c r="AP74" s="2"/>
       <c r="AQ74" s="4"/>
@@ -4372,17 +4933,37 @@
       <c r="AW74" s="2"/>
       <c r="AX74" s="2"/>
     </row>
-    <row r="75" spans="1:50" ht="16">
+    <row r="75" spans="1:50" ht="34">
       <c r="A75" s="2"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
+      <c r="B75" s="3">
+        <v>62</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E75" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Grenze NL/D – Kaldenkirchen – Mönchengladbach – Rheydt-Odenkirchen Teilmaßnahme Rheydt – Rheydt-Odenkirchen</v>
+      </c>
       <c r="F75" s="2"/>
-      <c r="G75" s="3"/>
+      <c r="G75" s="3" t="s">
+        <v>258</v>
+      </c>
       <c r="H75" s="3"/>
       <c r="I75" s="4"/>
       <c r="J75" s="1"/>
+      <c r="N75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB75">
+        <v>100</v>
+      </c>
       <c r="AO75" s="2"/>
       <c r="AP75" s="2"/>
       <c r="AQ75" s="4"/>
@@ -4394,19 +4975,33 @@
       <c r="AW75" s="2"/>
       <c r="AX75" s="2"/>
     </row>
-    <row r="76" spans="1:50" ht="16">
+    <row r="76" spans="1:50" ht="34">
       <c r="A76" s="2"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
+      <c r="B76" s="3">
+        <v>62</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E76" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Grenze NL/D – Kaldenkirchen – Mönchengladbach – Rheydt-Odenkirchen Teilmaßnahme Rheydt – Rheydt-Odenkirchen</v>
+      </c>
       <c r="F76" s="2"/>
-      <c r="G76" s="3"/>
+      <c r="G76" s="3" t="s">
+        <v>260</v>
+      </c>
       <c r="H76" s="3"/>
       <c r="I76" s="4"/>
       <c r="K76" s="1"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
+      <c r="Q76" t="b">
+        <v>1</v>
+      </c>
       <c r="AO76" s="2"/>
       <c r="AP76" s="2"/>
       <c r="AQ76" s="4"/>
@@ -4418,18 +5013,38 @@
       <c r="AW76" s="2"/>
       <c r="AX76" s="2"/>
     </row>
-    <row r="77" spans="1:50" ht="16">
+    <row r="77" spans="1:50" ht="119">
       <c r="A77" s="2"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
+      <c r="B77" s="3">
+        <v>70</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E77" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme NBS Zeppelinheim – Mannheim-Waldhof</v>
+      </c>
       <c r="F77" s="2"/>
-      <c r="G77" s="3"/>
+      <c r="G77" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="H77" s="3"/>
       <c r="I77" s="4"/>
+      <c r="J77" t="b">
+        <v>1</v>
+      </c>
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
+      <c r="AA77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB77">
+        <v>300</v>
+      </c>
       <c r="AO77" s="2"/>
       <c r="AP77" s="2"/>
       <c r="AQ77" s="4"/>
@@ -4443,16 +5058,30 @@
     </row>
     <row r="78" spans="1:50" ht="16">
       <c r="A78" s="2"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
+      <c r="B78" s="3">
+        <v>70</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E78" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme Verbindungskurve Klein-Gerau/Weiterstadt/Griesheim</v>
+      </c>
       <c r="F78" s="2"/>
-      <c r="G78" s="3"/>
+      <c r="G78" s="3" t="s">
+        <v>265</v>
+      </c>
       <c r="H78" s="3"/>
       <c r="I78" s="4"/>
       <c r="K78" s="1"/>
       <c r="O78" s="1"/>
+      <c r="Q78" t="b">
+        <v>1</v>
+      </c>
       <c r="U78" s="1"/>
       <c r="AO78" s="2"/>
       <c r="AP78" s="2"/>
@@ -4467,16 +5096,32 @@
     </row>
     <row r="79" spans="1:50" ht="16">
       <c r="A79" s="2"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
+      <c r="B79" s="3">
+        <v>70</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E79" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme zweites Gleis Mannheim Käfertal – Mannheim Rangierbahnhof</v>
+      </c>
       <c r="F79" s="2"/>
-      <c r="G79" s="3"/>
+      <c r="G79" s="3" t="s">
+        <v>268</v>
+      </c>
       <c r="H79" s="3"/>
       <c r="I79" s="4"/>
       <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
+      <c r="K79" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="N79" t="b">
+        <v>1</v>
+      </c>
       <c r="AO79" s="2"/>
       <c r="AP79" s="2"/>
       <c r="AQ79" s="4"/>
@@ -4490,16 +5135,43 @@
     </row>
     <row r="80" spans="1:50" ht="16">
       <c r="A80" s="2"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+      <c r="B80" s="3">
+        <v>70</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E80" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme ABS/NBS Molzau – Graben-Neudorf – Karlsruhe</v>
+      </c>
       <c r="F80" s="6"/>
-      <c r="G80" s="3"/>
+      <c r="G80" s="3" t="s">
+        <v>271</v>
+      </c>
       <c r="H80" s="3"/>
       <c r="I80" s="4"/>
-      <c r="K80" s="1"/>
-      <c r="O80" s="1"/>
+      <c r="J80" t="b">
+        <v>1</v>
+      </c>
+      <c r="K80" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O80" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB80">
+        <v>200</v>
+      </c>
       <c r="AO80" s="2"/>
       <c r="AP80" s="2"/>
       <c r="AQ80" s="4"/>
@@ -4511,16 +5183,33 @@
       <c r="AW80" s="2"/>
       <c r="AX80" s="2"/>
     </row>
-    <row r="81" spans="1:50" ht="16">
+    <row r="81" spans="1:50" ht="102">
       <c r="A81" s="2"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="B81" s="3">
+        <v>70</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E81" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme Wallauer Spange</v>
+      </c>
       <c r="F81" s="2"/>
-      <c r="G81" s="3"/>
+      <c r="G81" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="H81" s="3"/>
       <c r="I81" s="4"/>
+      <c r="J81" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q81" t="b">
+        <v>1</v>
+      </c>
       <c r="R81" s="1"/>
       <c r="AO81" s="2"/>
       <c r="AP81" s="2"/>
@@ -4535,16 +5224,31 @@
     </row>
     <row r="82" spans="1:50" ht="16">
       <c r="A82" s="2"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
+      <c r="B82" s="3">
+        <v>70</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E82" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme drittes Gleis Karlsruhe – Durmersheim</v>
+      </c>
       <c r="F82" s="2"/>
-      <c r="G82" s="3"/>
+      <c r="G82" s="3" t="s">
+        <v>278</v>
+      </c>
       <c r="H82" s="3"/>
       <c r="I82" s="4"/>
-      <c r="K82" s="1"/>
-      <c r="O82" s="1"/>
+      <c r="K82" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O82" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="AO82" s="2"/>
       <c r="AP82" s="2"/>
       <c r="AQ82" s="4"/>
@@ -4556,16 +5260,33 @@
       <c r="AW82" s="2"/>
       <c r="AX82" s="2"/>
     </row>
-    <row r="83" spans="1:50" ht="16">
+    <row r="83" spans="1:50" ht="34">
       <c r="A83" s="2"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
+      <c r="B83" s="3">
+        <v>70</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E83" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme drittes Gleis Groß Gerau-dornberg – Riedstadt-Goddelau</v>
+      </c>
       <c r="F83" s="2"/>
-      <c r="G83" s="3"/>
+      <c r="G83" s="3" t="s">
+        <v>281</v>
+      </c>
       <c r="H83" s="3"/>
       <c r="I83" s="4"/>
+      <c r="K83" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O83" t="b">
+        <v>1</v>
+      </c>
       <c r="S83" s="1"/>
       <c r="AO83" s="2"/>
       <c r="AP83" s="2"/>
@@ -4580,14 +5301,28 @@
     </row>
     <row r="84" spans="1:50" ht="16">
       <c r="A84" s="2"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
+      <c r="B84" s="3">
+        <v>70</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E84" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme KV-Profil P/C 400 Hagen – Siegen Ost Gbf, Au – Siegen – Siegen Ost Gbf, Siegen – Siegen-Weidenau</v>
+      </c>
       <c r="F84" s="2"/>
-      <c r="G84" s="3"/>
+      <c r="G84" s="3" t="s">
+        <v>284</v>
+      </c>
       <c r="H84" s="3"/>
       <c r="I84" s="4"/>
+      <c r="Z84" t="b">
+        <v>1</v>
+      </c>
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
       <c r="AO84" s="2"/>
@@ -4603,16 +5338,30 @@
     </row>
     <row r="85" spans="1:50" ht="16">
       <c r="A85" s="2"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+      <c r="B85" s="3">
+        <v>70</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E85" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme Blockverdichtung Krueztal – Siegen, Wetzlar – Gießen-Bergwald – Friedberg</v>
+      </c>
       <c r="F85" s="2"/>
-      <c r="G85" s="3"/>
+      <c r="G85" s="3" t="s">
+        <v>287</v>
+      </c>
       <c r="H85" s="3"/>
       <c r="I85" s="4"/>
       <c r="K85" s="1"/>
       <c r="P85" s="1"/>
+      <c r="X85" t="b">
+        <v>1</v>
+      </c>
       <c r="AO85" s="2"/>
       <c r="AP85" s="2"/>
       <c r="AQ85" s="4"/>
@@ -4626,15 +5375,31 @@
     </row>
     <row r="86" spans="1:50" ht="16">
       <c r="A86" s="2"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
+      <c r="B86" s="3">
+        <v>70</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E86" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme 10 zweites Gleis Blankenberg – Merten, Schladern – Rosbach</v>
+      </c>
       <c r="F86" s="2"/>
-      <c r="G86" s="3"/>
+      <c r="G86" s="3" t="s">
+        <v>290</v>
+      </c>
       <c r="H86" s="3"/>
       <c r="I86" s="4"/>
-      <c r="K86" s="1"/>
+      <c r="K86" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="N86" t="b">
+        <v>1</v>
+      </c>
       <c r="P86" s="1"/>
       <c r="AO86" s="2"/>
       <c r="AP86" s="2"/>
@@ -4649,16 +5414,30 @@
     </row>
     <row r="87" spans="1:50" ht="16">
       <c r="A87" s="2"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
+      <c r="B87" s="3">
+        <v>70</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E87" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme 11 höhenfreie Verknüpfung Friedberg, Großkrotzenburg</v>
+      </c>
       <c r="F87" s="2"/>
-      <c r="G87" s="3"/>
+      <c r="G87" s="3" t="s">
+        <v>293</v>
+      </c>
       <c r="H87" s="3"/>
       <c r="I87" s="4"/>
       <c r="K87" s="1"/>
       <c r="O87" s="1"/>
+      <c r="Y87" t="b">
+        <v>1</v>
+      </c>
       <c r="AO87" s="2"/>
       <c r="AP87" s="2"/>
       <c r="AQ87" s="4"/>
@@ -4670,16 +5449,33 @@
       <c r="AW87" s="2"/>
       <c r="AX87" s="2"/>
     </row>
-    <row r="88" spans="1:50" ht="16">
+    <row r="88" spans="1:50" ht="51">
       <c r="A88" s="2"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
+      <c r="B88" s="3">
+        <v>70</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E88" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mittelrhein: Zielnetz 1 Teilmaßnahme 12 viergleisiger Ausbau Frankfurt-Stadion – Zeppelinheim</v>
+      </c>
       <c r="F88" s="2"/>
-      <c r="G88" s="3"/>
+      <c r="G88" s="3" t="s">
+        <v>296</v>
+      </c>
       <c r="H88" s="3"/>
       <c r="I88" s="4"/>
+      <c r="K88" t="b">
+        <v>1</v>
+      </c>
+      <c r="P88" t="b">
+        <v>1</v>
+      </c>
       <c r="U88" s="1"/>
       <c r="V88" s="1"/>
       <c r="AO88" s="2"/>
@@ -4695,7 +5491,9 @@
     </row>
     <row r="89" spans="1:50" ht="16">
       <c r="A89" s="2"/>
-      <c r="B89" s="3"/>
+      <c r="B89" s="3">
+        <v>73</v>
+      </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>

</xml_diff>